<commit_message>
Update the issues of RS file
</commit_message>
<xml_diff>
--- a/ExchangeActiveSync/Docs/MS-ASRM/MS-ASRM_RequirementSpecification.xlsx
+++ b/ExchangeActiveSync/Docs/MS-ASRM/MS-ASRM_RequirementSpecification.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D042F46-BA54-430C-B711-0BBACC20F17B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB996058-59D7-4772-A58D-92CAC90FA5DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -3434,7 +3434,7 @@
     <t>MS-ASWBXML_R341</t>
   </si>
   <si>
-    <t>[In EditAllowed] Conversely, if [EditAllowed is set to FALSE and] composemail:ReplaceMime] is present[in a SmartReply command], the server will not attach the original rights-managed email message as an attachment.</t>
+    <t>[In EditAllowed] Conversely, if [EditAllowed is set to FALSE and] composemail:ReplaceMime is present[in a SmartReply command], the server will not attach the original rights-managed email message as an attachment.</t>
   </si>
 </sst>
 </file>
@@ -3733,21 +3733,6 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3772,1497 +3757,26 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="305">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -5599,6 +4113,1492 @@
         <vertAlign val="baseline"/>
         <name val="Calibri"/>
         <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
       </font>
     </dxf>
   </dxfs>
@@ -5730,34 +5730,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I495" tableType="xml" totalsRowShown="0" headerRowDxfId="304" dataDxfId="303" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I495" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I495" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="302">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="301">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="300">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="299">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="298">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="297">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="296">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="295">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="294">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -5766,12 +5766,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="293" dataDxfId="291" headerRowBorderDxfId="292" tableBorderDxfId="290" totalsRowBorderDxfId="289">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="288"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="287"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="286"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6101,8 +6101,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A397" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H401" sqref="H401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -6157,127 +6157,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -6290,12 +6290,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -6308,12 +6308,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -6326,12 +6326,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -6344,60 +6344,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -16028,7 +16028,7 @@
         <v>16</v>
       </c>
       <c r="H402" s="29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I402" s="37"/>
     </row>
@@ -18371,6 +18371,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -18378,1068 +18383,1063 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A403:B403 D403:I403 A468:B485 D468:I486 A20:H46 A34:I46 A101:I106 A112:I117 A135:I143 A149:I155 A173:I177 A183:I188 A194:I199 A205:I223 A229:I237 A243:I249 A255:I260 A280:I285 A306:I308 A314:I319 A339:I344 A65:I77 A83:I95 A161:I167 A47:B51 A96:B100 A78:B82 A60:B64 A52:I59 A118:B122 A107:B111 A130:B134 A144:B148 A156:B160 A168:B172 A178:B182 A189:B193 A200:B204 A224:B228 A238:B242 A250:B254 A261:B265 A266:I274 A275:B279 A286:B290 A291:I300 A301:B305 A309:B313 A320:B324 A325:I333 A334:B338 A345:B349 A350:I402 A487:I495 A404:I467 A123:I129 I20:I495">
-    <cfRule type="expression" dxfId="285" priority="331">
+    <cfRule type="expression" dxfId="304" priority="331">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="284" priority="332">
+    <cfRule type="expression" dxfId="303" priority="332">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="283" priority="339">
+    <cfRule type="expression" dxfId="302" priority="339">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A403:B403 D403:I403 A468:B485 D468:I486 A20:H46 A34:I46 A101:I106 A112:I117 A135:I143 A149:I155 A173:I177 A183:I188 A194:I199 A205:I223 A229:I237 A243:I249 A255:I260 A280:I285 A306:I308 A314:I319 A339:I344 A65:I77 A83:I95 A161:I167 A47:B51 A96:B100 A78:B82 A60:B64 A52:I59 A118:B122 A107:B111 A130:B134 A144:B148 A156:B160 A168:B172 A178:B182 A189:B193 A200:B204 A224:B228 A238:B242 A250:B254 A261:B265 A266:I274 A275:B279 A286:B290 A291:I300 A301:B305 A309:B313 A320:B324 A325:I333 A334:B338 A345:B349 A350:I402 A487:I495 A404:I467 A123:I129 I20:I495">
-    <cfRule type="expression" dxfId="282" priority="285">
+    <cfRule type="expression" dxfId="301" priority="285">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="281" priority="286">
+    <cfRule type="expression" dxfId="300" priority="286">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="280" priority="287">
+    <cfRule type="expression" dxfId="299" priority="287">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F46 F65:F77 F83:F95 F101:F106 F112:F117 F135:F143 F149:F155 F173:F177 F183:F188 F194:F199 F205:F223 F229:F237 F243:F249 F255:F260 F280:F285 F306:F308 F314:F319 F339:F344 F161:F167 F52:F59 F266:F274 F291:F300 F325:F333 F350:F495 F123:F129">
-    <cfRule type="expression" dxfId="279" priority="291">
+    <cfRule type="expression" dxfId="298" priority="291">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="278" priority="292">
+    <cfRule type="expression" dxfId="297" priority="292">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C403">
-    <cfRule type="expression" dxfId="277" priority="276">
+    <cfRule type="expression" dxfId="296" priority="276">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="276" priority="277">
+    <cfRule type="expression" dxfId="295" priority="277">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="275" priority="278">
+    <cfRule type="expression" dxfId="294" priority="278">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C403">
-    <cfRule type="expression" dxfId="274" priority="273">
+    <cfRule type="expression" dxfId="293" priority="273">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="273" priority="274">
+    <cfRule type="expression" dxfId="292" priority="274">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="272" priority="275">
+    <cfRule type="expression" dxfId="291" priority="275">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A486:B486">
-    <cfRule type="expression" dxfId="271" priority="267">
+    <cfRule type="expression" dxfId="290" priority="267">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="270" priority="268">
+    <cfRule type="expression" dxfId="289" priority="268">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="269" priority="269">
+    <cfRule type="expression" dxfId="288" priority="269">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A486:B486">
-    <cfRule type="expression" dxfId="268" priority="270">
+    <cfRule type="expression" dxfId="287" priority="270">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="267" priority="271">
+    <cfRule type="expression" dxfId="286" priority="271">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="266" priority="272">
+    <cfRule type="expression" dxfId="285" priority="272">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C468:C486">
-    <cfRule type="expression" dxfId="265" priority="264">
+    <cfRule type="expression" dxfId="284" priority="264">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="264" priority="265">
+    <cfRule type="expression" dxfId="283" priority="265">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="263" priority="266">
+    <cfRule type="expression" dxfId="282" priority="266">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C468:C486">
-    <cfRule type="expression" dxfId="262" priority="261">
+    <cfRule type="expression" dxfId="281" priority="261">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="261" priority="262">
+    <cfRule type="expression" dxfId="280" priority="262">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="260" priority="263">
+    <cfRule type="expression" dxfId="279" priority="263">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47:D51">
-    <cfRule type="expression" dxfId="259" priority="258">
+    <cfRule type="expression" dxfId="278" priority="258">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="258" priority="259">
+    <cfRule type="expression" dxfId="277" priority="259">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="257" priority="260">
+    <cfRule type="expression" dxfId="276" priority="260">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47:D51">
-    <cfRule type="expression" dxfId="256" priority="255">
+    <cfRule type="expression" dxfId="275" priority="255">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="255" priority="256">
+    <cfRule type="expression" dxfId="274" priority="256">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="254" priority="257">
+    <cfRule type="expression" dxfId="273" priority="257">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C51">
-    <cfRule type="expression" dxfId="253" priority="252">
+    <cfRule type="expression" dxfId="272" priority="252">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="252" priority="253">
+    <cfRule type="expression" dxfId="271" priority="253">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="251" priority="254">
+    <cfRule type="expression" dxfId="270" priority="254">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C51">
-    <cfRule type="expression" dxfId="250" priority="249">
+    <cfRule type="expression" dxfId="269" priority="249">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="249" priority="250">
+    <cfRule type="expression" dxfId="268" priority="250">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="248" priority="251">
+    <cfRule type="expression" dxfId="267" priority="251">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47:H51">
-    <cfRule type="expression" dxfId="247" priority="246">
+    <cfRule type="expression" dxfId="266" priority="246">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="246" priority="247">
+    <cfRule type="expression" dxfId="265" priority="247">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="245" priority="248">
+    <cfRule type="expression" dxfId="264" priority="248">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47:H51">
-    <cfRule type="expression" dxfId="244" priority="241">
+    <cfRule type="expression" dxfId="263" priority="241">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="243" priority="242">
+    <cfRule type="expression" dxfId="262" priority="242">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="242" priority="243">
+    <cfRule type="expression" dxfId="261" priority="243">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:F51">
-    <cfRule type="expression" dxfId="241" priority="244">
+    <cfRule type="expression" dxfId="260" priority="244">
       <formula>NOT(VLOOKUP(F47,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="240" priority="245">
+    <cfRule type="expression" dxfId="259" priority="245">
       <formula>(VLOOKUP(F47,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78:D82 D60:D64">
-    <cfRule type="expression" dxfId="239" priority="238">
+    <cfRule type="expression" dxfId="258" priority="238">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="238" priority="239">
+    <cfRule type="expression" dxfId="257" priority="239">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="237" priority="240">
+    <cfRule type="expression" dxfId="256" priority="240">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78:D82 D60:D64">
-    <cfRule type="expression" dxfId="236" priority="235">
+    <cfRule type="expression" dxfId="255" priority="235">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="235" priority="236">
+    <cfRule type="expression" dxfId="254" priority="236">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="234" priority="237">
+    <cfRule type="expression" dxfId="253" priority="237">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C64 C78:C82">
-    <cfRule type="expression" dxfId="233" priority="232">
+    <cfRule type="expression" dxfId="252" priority="232">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="232" priority="233">
+    <cfRule type="expression" dxfId="251" priority="233">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="231" priority="234">
+    <cfRule type="expression" dxfId="250" priority="234">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C64 C78:C82">
-    <cfRule type="expression" dxfId="230" priority="229">
+    <cfRule type="expression" dxfId="249" priority="229">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="229" priority="230">
+    <cfRule type="expression" dxfId="248" priority="230">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="228" priority="231">
+    <cfRule type="expression" dxfId="247" priority="231">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:H82 E60:H64">
-    <cfRule type="expression" dxfId="227" priority="226">
+    <cfRule type="expression" dxfId="246" priority="226">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="226" priority="227">
+    <cfRule type="expression" dxfId="245" priority="227">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="225" priority="228">
+    <cfRule type="expression" dxfId="244" priority="228">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:H82 E60:H64">
-    <cfRule type="expression" dxfId="224" priority="221">
+    <cfRule type="expression" dxfId="243" priority="221">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="223" priority="222">
+    <cfRule type="expression" dxfId="242" priority="222">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="222" priority="223">
+    <cfRule type="expression" dxfId="241" priority="223">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F78:F82 F60:F64">
-    <cfRule type="expression" dxfId="221" priority="224">
+    <cfRule type="expression" dxfId="240" priority="224">
       <formula>NOT(VLOOKUP(F60,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="220" priority="225">
+    <cfRule type="expression" dxfId="239" priority="225">
       <formula>(VLOOKUP(F60,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D107:D111 D96:D100">
-    <cfRule type="expression" dxfId="219" priority="218">
+    <cfRule type="expression" dxfId="238" priority="218">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="218" priority="219">
+    <cfRule type="expression" dxfId="237" priority="219">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="217" priority="220">
+    <cfRule type="expression" dxfId="236" priority="220">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D107:D111 D96:D100">
-    <cfRule type="expression" dxfId="216" priority="215">
+    <cfRule type="expression" dxfId="235" priority="215">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="215" priority="216">
+    <cfRule type="expression" dxfId="234" priority="216">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="214" priority="217">
+    <cfRule type="expression" dxfId="233" priority="217">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C96:C100 C107:C111">
-    <cfRule type="expression" dxfId="213" priority="212">
+    <cfRule type="expression" dxfId="232" priority="212">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="212" priority="213">
+    <cfRule type="expression" dxfId="231" priority="213">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="211" priority="214">
+    <cfRule type="expression" dxfId="230" priority="214">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C96:C100 C107:C111">
-    <cfRule type="expression" dxfId="210" priority="209">
+    <cfRule type="expression" dxfId="229" priority="209">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="209" priority="210">
+    <cfRule type="expression" dxfId="228" priority="210">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="208" priority="211">
+    <cfRule type="expression" dxfId="227" priority="211">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E96:H100 E107:H111">
-    <cfRule type="expression" dxfId="207" priority="206">
+    <cfRule type="expression" dxfId="226" priority="206">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="206" priority="207">
+    <cfRule type="expression" dxfId="225" priority="207">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="205" priority="208">
+    <cfRule type="expression" dxfId="224" priority="208">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E96:H100 E107:H111">
-    <cfRule type="expression" dxfId="204" priority="201">
+    <cfRule type="expression" dxfId="223" priority="201">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="203" priority="202">
+    <cfRule type="expression" dxfId="222" priority="202">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="202" priority="203">
+    <cfRule type="expression" dxfId="221" priority="203">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F96:F100 F107:F111">
-    <cfRule type="expression" dxfId="201" priority="204">
+    <cfRule type="expression" dxfId="220" priority="204">
       <formula>NOT(VLOOKUP(F96,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="205">
+    <cfRule type="expression" dxfId="219" priority="205">
       <formula>(VLOOKUP(F96,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D130:D134 D118:D122">
-    <cfRule type="expression" dxfId="199" priority="198">
+    <cfRule type="expression" dxfId="218" priority="198">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="198" priority="199">
+    <cfRule type="expression" dxfId="217" priority="199">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="197" priority="200">
+    <cfRule type="expression" dxfId="216" priority="200">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D130:D134 D118:D122">
-    <cfRule type="expression" dxfId="196" priority="195">
+    <cfRule type="expression" dxfId="215" priority="195">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="196">
+    <cfRule type="expression" dxfId="214" priority="196">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="194" priority="197">
+    <cfRule type="expression" dxfId="213" priority="197">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C118:C122 C130:C134">
-    <cfRule type="expression" dxfId="193" priority="192">
+    <cfRule type="expression" dxfId="212" priority="192">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="193">
+    <cfRule type="expression" dxfId="211" priority="193">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="191" priority="194">
+    <cfRule type="expression" dxfId="210" priority="194">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C118:C122 C130:C134">
-    <cfRule type="expression" dxfId="190" priority="189">
+    <cfRule type="expression" dxfId="209" priority="189">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="189" priority="190">
+    <cfRule type="expression" dxfId="208" priority="190">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="188" priority="191">
+    <cfRule type="expression" dxfId="207" priority="191">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130:H134 E118:H122">
-    <cfRule type="expression" dxfId="187" priority="186">
+    <cfRule type="expression" dxfId="206" priority="186">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="187">
+    <cfRule type="expression" dxfId="205" priority="187">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="185" priority="188">
+    <cfRule type="expression" dxfId="204" priority="188">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130:H134 E118:H122">
-    <cfRule type="expression" dxfId="184" priority="181">
+    <cfRule type="expression" dxfId="203" priority="181">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="183" priority="182">
+    <cfRule type="expression" dxfId="202" priority="182">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="182" priority="183">
+    <cfRule type="expression" dxfId="201" priority="183">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F130:F134 F118:F122">
-    <cfRule type="expression" dxfId="181" priority="184">
+    <cfRule type="expression" dxfId="200" priority="184">
       <formula>NOT(VLOOKUP(F118,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="185">
+    <cfRule type="expression" dxfId="199" priority="185">
       <formula>(VLOOKUP(F118,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D156:D160 D144:D148">
-    <cfRule type="expression" dxfId="179" priority="178">
+    <cfRule type="expression" dxfId="198" priority="178">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="179">
+    <cfRule type="expression" dxfId="197" priority="179">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="177" priority="180">
+    <cfRule type="expression" dxfId="196" priority="180">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D156:D160 D144:D148">
-    <cfRule type="expression" dxfId="176" priority="175">
+    <cfRule type="expression" dxfId="195" priority="175">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="175" priority="176">
+    <cfRule type="expression" dxfId="194" priority="176">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="177">
+    <cfRule type="expression" dxfId="193" priority="177">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C144:C148 C156:C160">
-    <cfRule type="expression" dxfId="173" priority="172">
+    <cfRule type="expression" dxfId="192" priority="172">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="173">
+    <cfRule type="expression" dxfId="191" priority="173">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="174">
+    <cfRule type="expression" dxfId="190" priority="174">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C144:C148 C156:C160">
-    <cfRule type="expression" dxfId="170" priority="169">
+    <cfRule type="expression" dxfId="189" priority="169">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="170">
+    <cfRule type="expression" dxfId="188" priority="170">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="171">
+    <cfRule type="expression" dxfId="187" priority="171">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E156:H160 E144:H148">
-    <cfRule type="expression" dxfId="167" priority="166">
+    <cfRule type="expression" dxfId="186" priority="166">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="167">
+    <cfRule type="expression" dxfId="185" priority="167">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="168">
+    <cfRule type="expression" dxfId="184" priority="168">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E156:H160 E144:H148">
-    <cfRule type="expression" dxfId="164" priority="161">
+    <cfRule type="expression" dxfId="183" priority="161">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="162">
+    <cfRule type="expression" dxfId="182" priority="162">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="163">
+    <cfRule type="expression" dxfId="181" priority="163">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F156:F160 F144:F148">
-    <cfRule type="expression" dxfId="161" priority="164">
+    <cfRule type="expression" dxfId="180" priority="164">
       <formula>NOT(VLOOKUP(F144,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="165">
+    <cfRule type="expression" dxfId="179" priority="165">
       <formula>(VLOOKUP(F144,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D178:D182 D168:D172">
-    <cfRule type="expression" dxfId="159" priority="158">
+    <cfRule type="expression" dxfId="178" priority="158">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="159">
+    <cfRule type="expression" dxfId="177" priority="159">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="160">
+    <cfRule type="expression" dxfId="176" priority="160">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D178:D182 D168:D172">
-    <cfRule type="expression" dxfId="156" priority="155">
+    <cfRule type="expression" dxfId="175" priority="155">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="156">
+    <cfRule type="expression" dxfId="174" priority="156">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="157">
+    <cfRule type="expression" dxfId="173" priority="157">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C168:C172 C178:C182">
-    <cfRule type="expression" dxfId="153" priority="152">
+    <cfRule type="expression" dxfId="172" priority="152">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="153">
+    <cfRule type="expression" dxfId="171" priority="153">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="154">
+    <cfRule type="expression" dxfId="170" priority="154">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C168:C172 C178:C182">
-    <cfRule type="expression" dxfId="150" priority="149">
+    <cfRule type="expression" dxfId="169" priority="149">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="150">
+    <cfRule type="expression" dxfId="168" priority="150">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="151">
+    <cfRule type="expression" dxfId="167" priority="151">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E168:H172 E178:H182">
-    <cfRule type="expression" dxfId="147" priority="146">
+    <cfRule type="expression" dxfId="166" priority="146">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="147">
+    <cfRule type="expression" dxfId="165" priority="147">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="148">
+    <cfRule type="expression" dxfId="164" priority="148">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E168:H172 E178:H182">
-    <cfRule type="expression" dxfId="144" priority="141">
+    <cfRule type="expression" dxfId="163" priority="141">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="142">
+    <cfRule type="expression" dxfId="162" priority="142">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="143">
+    <cfRule type="expression" dxfId="161" priority="143">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F168:F172 F178:F182">
-    <cfRule type="expression" dxfId="141" priority="144">
+    <cfRule type="expression" dxfId="160" priority="144">
       <formula>NOT(VLOOKUP(F168,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="145">
+    <cfRule type="expression" dxfId="159" priority="145">
       <formula>(VLOOKUP(F168,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D200:D204 D189:D193">
-    <cfRule type="expression" dxfId="139" priority="138">
+    <cfRule type="expression" dxfId="158" priority="138">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="139">
+    <cfRule type="expression" dxfId="157" priority="139">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="140">
+    <cfRule type="expression" dxfId="156" priority="140">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D200:D204 D189:D193">
-    <cfRule type="expression" dxfId="136" priority="135">
+    <cfRule type="expression" dxfId="155" priority="135">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="136">
+    <cfRule type="expression" dxfId="154" priority="136">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="137">
+    <cfRule type="expression" dxfId="153" priority="137">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C189:C193 C200:C204">
-    <cfRule type="expression" dxfId="133" priority="132">
+    <cfRule type="expression" dxfId="152" priority="132">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="133">
+    <cfRule type="expression" dxfId="151" priority="133">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="134">
+    <cfRule type="expression" dxfId="150" priority="134">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C189:C193 C200:C204">
-    <cfRule type="expression" dxfId="130" priority="129">
+    <cfRule type="expression" dxfId="149" priority="129">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="130">
+    <cfRule type="expression" dxfId="148" priority="130">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="131">
+    <cfRule type="expression" dxfId="147" priority="131">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E200:H204 E189:H193">
-    <cfRule type="expression" dxfId="127" priority="126">
+    <cfRule type="expression" dxfId="146" priority="126">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="127">
+    <cfRule type="expression" dxfId="145" priority="127">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="128">
+    <cfRule type="expression" dxfId="144" priority="128">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E200:H204 E189:H193">
-    <cfRule type="expression" dxfId="124" priority="121">
+    <cfRule type="expression" dxfId="143" priority="121">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="122">
+    <cfRule type="expression" dxfId="142" priority="122">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="123">
+    <cfRule type="expression" dxfId="141" priority="123">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F200:F204 F189:F193">
-    <cfRule type="expression" dxfId="121" priority="124">
+    <cfRule type="expression" dxfId="140" priority="124">
       <formula>NOT(VLOOKUP(F189,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="125">
+    <cfRule type="expression" dxfId="139" priority="125">
       <formula>(VLOOKUP(F189,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D238:D242 D224:D228">
-    <cfRule type="expression" dxfId="119" priority="118">
+    <cfRule type="expression" dxfId="138" priority="118">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="119">
+    <cfRule type="expression" dxfId="137" priority="119">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="120">
+    <cfRule type="expression" dxfId="136" priority="120">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D238:D242 D224:D228">
-    <cfRule type="expression" dxfId="116" priority="115">
+    <cfRule type="expression" dxfId="135" priority="115">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="116">
+    <cfRule type="expression" dxfId="134" priority="116">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="117">
+    <cfRule type="expression" dxfId="133" priority="117">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C224:C228 C238:C242">
-    <cfRule type="expression" dxfId="113" priority="112">
+    <cfRule type="expression" dxfId="132" priority="112">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="113">
+    <cfRule type="expression" dxfId="131" priority="113">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="114">
+    <cfRule type="expression" dxfId="130" priority="114">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C224:C228 C238:C242">
-    <cfRule type="expression" dxfId="110" priority="109">
+    <cfRule type="expression" dxfId="129" priority="109">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="110">
+    <cfRule type="expression" dxfId="128" priority="110">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="111">
+    <cfRule type="expression" dxfId="127" priority="111">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E224:H228 E238:H242">
-    <cfRule type="expression" dxfId="107" priority="106">
+    <cfRule type="expression" dxfId="126" priority="106">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="107">
+    <cfRule type="expression" dxfId="125" priority="107">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="108">
+    <cfRule type="expression" dxfId="124" priority="108">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E224:H228 E238:H242">
-    <cfRule type="expression" dxfId="104" priority="101">
+    <cfRule type="expression" dxfId="123" priority="101">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="102">
+    <cfRule type="expression" dxfId="122" priority="102">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="103">
+    <cfRule type="expression" dxfId="121" priority="103">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F224:F228 F238:F242">
-    <cfRule type="expression" dxfId="101" priority="104">
+    <cfRule type="expression" dxfId="120" priority="104">
       <formula>NOT(VLOOKUP(F224,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="105">
+    <cfRule type="expression" dxfId="119" priority="105">
       <formula>(VLOOKUP(F224,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D261:D265 D250:D254">
-    <cfRule type="expression" dxfId="99" priority="98">
+    <cfRule type="expression" dxfId="118" priority="98">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="99">
+    <cfRule type="expression" dxfId="117" priority="99">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="100">
+    <cfRule type="expression" dxfId="116" priority="100">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D261:D265 D250:D254">
-    <cfRule type="expression" dxfId="96" priority="95">
+    <cfRule type="expression" dxfId="115" priority="95">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="96">
+    <cfRule type="expression" dxfId="114" priority="96">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="97">
+    <cfRule type="expression" dxfId="113" priority="97">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C250:C254 C261:C265">
-    <cfRule type="expression" dxfId="93" priority="92">
+    <cfRule type="expression" dxfId="112" priority="92">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="93">
+    <cfRule type="expression" dxfId="111" priority="93">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="94">
+    <cfRule type="expression" dxfId="110" priority="94">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C250:C254 C261:C265">
-    <cfRule type="expression" dxfId="90" priority="89">
+    <cfRule type="expression" dxfId="109" priority="89">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="90">
+    <cfRule type="expression" dxfId="108" priority="90">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="91">
+    <cfRule type="expression" dxfId="107" priority="91">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E250:H254 E261:H265">
-    <cfRule type="expression" dxfId="87" priority="86">
+    <cfRule type="expression" dxfId="106" priority="86">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="87">
+    <cfRule type="expression" dxfId="105" priority="87">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="88">
+    <cfRule type="expression" dxfId="104" priority="88">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E250:H254 E261:H265">
-    <cfRule type="expression" dxfId="84" priority="81">
+    <cfRule type="expression" dxfId="103" priority="81">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="82">
+    <cfRule type="expression" dxfId="102" priority="82">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="83">
+    <cfRule type="expression" dxfId="101" priority="83">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F250:F254 F261:F265">
-    <cfRule type="expression" dxfId="81" priority="84">
+    <cfRule type="expression" dxfId="100" priority="84">
       <formula>NOT(VLOOKUP(F250,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="85">
+    <cfRule type="expression" dxfId="99" priority="85">
       <formula>(VLOOKUP(F250,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D286:D290 D275:D279">
-    <cfRule type="expression" dxfId="79" priority="78">
+    <cfRule type="expression" dxfId="98" priority="78">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="79">
+    <cfRule type="expression" dxfId="97" priority="79">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="80">
+    <cfRule type="expression" dxfId="96" priority="80">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D286:D290 D275:D279">
-    <cfRule type="expression" dxfId="76" priority="75">
+    <cfRule type="expression" dxfId="95" priority="75">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="76">
+    <cfRule type="expression" dxfId="94" priority="76">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="77">
+    <cfRule type="expression" dxfId="93" priority="77">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C275:C279 C286:C290">
-    <cfRule type="expression" dxfId="73" priority="72">
+    <cfRule type="expression" dxfId="92" priority="72">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="73">
+    <cfRule type="expression" dxfId="91" priority="73">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="74">
+    <cfRule type="expression" dxfId="90" priority="74">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C275:C279 C286:C290">
-    <cfRule type="expression" dxfId="70" priority="69">
+    <cfRule type="expression" dxfId="89" priority="69">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="70">
+    <cfRule type="expression" dxfId="88" priority="70">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="71">
+    <cfRule type="expression" dxfId="87" priority="71">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E275:H279 E286:H290">
-    <cfRule type="expression" dxfId="67" priority="66">
+    <cfRule type="expression" dxfId="86" priority="66">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="67">
+    <cfRule type="expression" dxfId="85" priority="67">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="68">
+    <cfRule type="expression" dxfId="84" priority="68">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E275:H279 E286:H290">
-    <cfRule type="expression" dxfId="64" priority="61">
+    <cfRule type="expression" dxfId="83" priority="61">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="62">
+    <cfRule type="expression" dxfId="82" priority="62">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="63">
+    <cfRule type="expression" dxfId="81" priority="63">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F275:F279 F286:F290">
-    <cfRule type="expression" dxfId="61" priority="64">
+    <cfRule type="expression" dxfId="80" priority="64">
       <formula>NOT(VLOOKUP(F275,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="65">
+    <cfRule type="expression" dxfId="79" priority="65">
       <formula>(VLOOKUP(F275,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D309:D313 D301:D305">
-    <cfRule type="expression" dxfId="59" priority="58">
+    <cfRule type="expression" dxfId="78" priority="58">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="59">
+    <cfRule type="expression" dxfId="77" priority="59">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="60">
+    <cfRule type="expression" dxfId="76" priority="60">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D309:D313 D301:D305">
-    <cfRule type="expression" dxfId="56" priority="55">
+    <cfRule type="expression" dxfId="75" priority="55">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="56">
+    <cfRule type="expression" dxfId="74" priority="56">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="57">
+    <cfRule type="expression" dxfId="73" priority="57">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C301:C305 C309:C313">
-    <cfRule type="expression" dxfId="53" priority="52">
+    <cfRule type="expression" dxfId="72" priority="52">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="53">
+    <cfRule type="expression" dxfId="71" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="54">
+    <cfRule type="expression" dxfId="70" priority="54">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C301:C305 C309:C313">
-    <cfRule type="expression" dxfId="50" priority="49">
+    <cfRule type="expression" dxfId="69" priority="49">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="50">
+    <cfRule type="expression" dxfId="68" priority="50">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="51">
+    <cfRule type="expression" dxfId="67" priority="51">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E301:H305 E309:H313">
-    <cfRule type="expression" dxfId="47" priority="46">
+    <cfRule type="expression" dxfId="66" priority="46">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="47">
+    <cfRule type="expression" dxfId="65" priority="47">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="48">
+    <cfRule type="expression" dxfId="64" priority="48">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E301:H305 E309:H313">
-    <cfRule type="expression" dxfId="44" priority="41">
+    <cfRule type="expression" dxfId="63" priority="41">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="42">
+    <cfRule type="expression" dxfId="62" priority="42">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="43">
+    <cfRule type="expression" dxfId="61" priority="43">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F301:F305 F309:F313">
-    <cfRule type="expression" dxfId="41" priority="44">
+    <cfRule type="expression" dxfId="60" priority="44">
       <formula>NOT(VLOOKUP(F301,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="45">
+    <cfRule type="expression" dxfId="59" priority="45">
       <formula>(VLOOKUP(F301,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D334:D338 D320:D324">
-    <cfRule type="expression" dxfId="39" priority="38">
+    <cfRule type="expression" dxfId="58" priority="38">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="39">
+    <cfRule type="expression" dxfId="57" priority="39">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="40">
+    <cfRule type="expression" dxfId="56" priority="40">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D334:D338 D320:D324">
-    <cfRule type="expression" dxfId="36" priority="35">
+    <cfRule type="expression" dxfId="55" priority="35">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="36">
+    <cfRule type="expression" dxfId="54" priority="36">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="37">
+    <cfRule type="expression" dxfId="53" priority="37">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C320:C324 C334:C338">
-    <cfRule type="expression" dxfId="33" priority="32">
+    <cfRule type="expression" dxfId="52" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="33">
+    <cfRule type="expression" dxfId="51" priority="33">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="34">
+    <cfRule type="expression" dxfId="50" priority="34">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C320:C324 C334:C338">
-    <cfRule type="expression" dxfId="30" priority="29">
+    <cfRule type="expression" dxfId="49" priority="29">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="30">
+    <cfRule type="expression" dxfId="48" priority="30">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="31">
+    <cfRule type="expression" dxfId="47" priority="31">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E320:H324 E334:H338">
-    <cfRule type="expression" dxfId="27" priority="26">
+    <cfRule type="expression" dxfId="46" priority="26">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="27">
+    <cfRule type="expression" dxfId="45" priority="27">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="28">
+    <cfRule type="expression" dxfId="44" priority="28">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E320:H324 E334:H338">
-    <cfRule type="expression" dxfId="24" priority="21">
+    <cfRule type="expression" dxfId="43" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="22">
+    <cfRule type="expression" dxfId="42" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="23">
+    <cfRule type="expression" dxfId="41" priority="23">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F320:F324 F334:F338">
-    <cfRule type="expression" dxfId="21" priority="24">
+    <cfRule type="expression" dxfId="40" priority="24">
       <formula>NOT(VLOOKUP(F320,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="25">
+    <cfRule type="expression" dxfId="39" priority="25">
       <formula>(VLOOKUP(F320,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D345:D349">
-    <cfRule type="expression" dxfId="19" priority="18">
+    <cfRule type="expression" dxfId="38" priority="18">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="37" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="20">
+    <cfRule type="expression" dxfId="36" priority="20">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D345:D349">
-    <cfRule type="expression" dxfId="16" priority="15">
+    <cfRule type="expression" dxfId="35" priority="15">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="34" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="17">
+    <cfRule type="expression" dxfId="33" priority="17">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C345:C349">
-    <cfRule type="expression" dxfId="13" priority="12">
+    <cfRule type="expression" dxfId="32" priority="12">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="31" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="14">
+    <cfRule type="expression" dxfId="30" priority="14">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C345:C349">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="29" priority="9">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="28" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="27" priority="11">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E345:H349">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="26" priority="6">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="25" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E345:H349">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F345:F349">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>NOT(VLOOKUP(F345,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>(VLOOKUP(F345,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19477,15 +19477,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -19534,6 +19525,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
@@ -19541,14 +19541,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19559,6 +19551,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update the RS version of MS-ASRM
</commit_message>
<xml_diff>
--- a/ExchangeActiveSync/Docs/MS-ASRM/MS-ASRM_RequirementSpecification.xlsx
+++ b/ExchangeActiveSync/Docs/MS-ASRM/MS-ASRM_RequirementSpecification.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB996058-59D7-4772-A58D-92CAC90FA5DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4145EABB-8E85-46BC-8013-805E66049144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2358,9 +2358,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>6.0</t>
-  </si>
-  <si>
     <t>[In EditAllowed] if the value is FALSE (0), the email cannot be modified by the user.</t>
   </si>
   <si>
@@ -3435,6 +3432,9 @@
   </si>
   <si>
     <t>[In EditAllowed] Conversely, if [EditAllowed is set to FALSE and] composemail:ReplaceMime is present[in a SmartReply command], the server will not attach the original rights-managed email message as an attachment.</t>
+  </si>
+  <si>
+    <t>10.0</t>
   </si>
 </sst>
 </file>
@@ -3733,6 +3733,21 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3756,21 +3771,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6101,8 +6101,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A397" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H401" sqref="H401"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -6146,138 +6146,138 @@
         <v>25</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>698</v>
+        <v>1055</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>697</v>
       </c>
       <c r="F3" s="12">
-        <v>42185</v>
+        <v>43374</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -6290,12 +6290,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -6308,12 +6308,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -6326,12 +6326,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -6344,60 +6344,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -6464,7 +6464,7 @@
         <v>388</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22" t="s">
@@ -6689,7 +6689,7 @@
         <v>391</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22" t="s">
@@ -6739,7 +6739,7 @@
         <v>391</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22" t="s">
@@ -6814,7 +6814,7 @@
         <v>391</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="29" t="s">
@@ -6839,7 +6839,7 @@
         <v>391</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D36" s="29"/>
       <c r="E36" s="29" t="s">
@@ -6864,7 +6864,7 @@
         <v>391</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="D37" s="29"/>
       <c r="E37" s="29" t="s">
@@ -7014,7 +7014,7 @@
         <v>392</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="29" t="s">
@@ -7108,13 +7108,13 @@
     </row>
     <row r="47" spans="1:9" ht="30">
       <c r="A47" s="22" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B47" s="30" t="s">
         <v>392</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="22" t="s">
@@ -7133,13 +7133,13 @@
     </row>
     <row r="48" spans="1:9" ht="30">
       <c r="A48" s="22" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B48" s="30" t="s">
         <v>392</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="22" t="s">
@@ -7158,13 +7158,13 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="22" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B49" s="30" t="s">
         <v>392</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="22" t="s">
@@ -7183,13 +7183,13 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="22" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B50" s="30" t="s">
         <v>392</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D50" s="22"/>
       <c r="E50" s="22" t="s">
@@ -7208,13 +7208,13 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="22" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B51" s="30" t="s">
         <v>392</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D51" s="36"/>
       <c r="E51" s="22" t="s">
@@ -7314,7 +7314,7 @@
         <v>393</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="29" t="s">
@@ -7333,13 +7333,13 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="22" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B56" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D56" s="36"/>
       <c r="E56" s="29" t="s">
@@ -7437,13 +7437,13 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="22" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B60" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D60" s="22"/>
       <c r="E60" s="22" t="s">
@@ -7462,13 +7462,13 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="22" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B61" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D61" s="22"/>
       <c r="E61" s="22" t="s">
@@ -7487,13 +7487,13 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="22" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B62" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D62" s="22"/>
       <c r="E62" s="22" t="s">
@@ -7512,13 +7512,13 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="22" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B63" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D63" s="22"/>
       <c r="E63" s="22" t="s">
@@ -7537,13 +7537,13 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="22" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B64" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D64" s="36"/>
       <c r="E64" s="22" t="s">
@@ -7643,7 +7643,7 @@
         <v>394</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="29" t="s">
@@ -7662,13 +7662,13 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="22" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B69" s="30" t="s">
         <v>394</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="29" t="s">
@@ -7687,13 +7687,13 @@
     </row>
     <row r="70" spans="1:9" ht="30">
       <c r="A70" s="22" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B70" s="30" t="s">
         <v>394</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="29" t="s">
@@ -7718,7 +7718,7 @@
         <v>394</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="D71" s="29"/>
       <c r="E71" s="29" t="s">
@@ -7768,7 +7768,7 @@
         <v>394</v>
       </c>
       <c r="C73" s="20" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="29" t="s">
@@ -7793,7 +7793,7 @@
         <v>394</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D74" s="29"/>
       <c r="E74" s="29" t="s">
@@ -7843,7 +7843,7 @@
         <v>394</v>
       </c>
       <c r="C76" s="20" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D76" s="29"/>
       <c r="E76" s="29" t="s">
@@ -7887,13 +7887,13 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="22" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B78" s="30" t="s">
         <v>394</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D78" s="22"/>
       <c r="E78" s="22" t="s">
@@ -7912,13 +7912,13 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="22" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B79" s="30" t="s">
         <v>394</v>
       </c>
       <c r="C79" s="20" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D79" s="22"/>
       <c r="E79" s="22" t="s">
@@ -7937,13 +7937,13 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="22" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B80" s="30" t="s">
         <v>394</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D80" s="22"/>
       <c r="E80" s="22" t="s">
@@ -7962,13 +7962,13 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="22" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B81" s="30" t="s">
         <v>394</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D81" s="22"/>
       <c r="E81" s="22" t="s">
@@ -7987,13 +7987,13 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="22" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B82" s="30" t="s">
         <v>394</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="D82" s="22"/>
       <c r="E82" s="22" t="s">
@@ -8093,7 +8093,7 @@
         <v>395</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D86" s="29"/>
       <c r="E86" s="29" t="s">
@@ -8118,7 +8118,7 @@
         <v>395</v>
       </c>
       <c r="C87" s="20" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="D87" s="29"/>
       <c r="E87" s="29" t="s">
@@ -8143,7 +8143,7 @@
         <v>395</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D88" s="29"/>
       <c r="E88" s="29" t="s">
@@ -8168,7 +8168,7 @@
         <v>395</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="D89" s="29"/>
       <c r="E89" s="29" t="s">
@@ -8193,7 +8193,7 @@
         <v>395</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D90" s="29"/>
       <c r="E90" s="29" t="s">
@@ -8218,7 +8218,7 @@
         <v>395</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D91" s="29"/>
       <c r="E91" s="29" t="s">
@@ -8243,7 +8243,7 @@
         <v>395</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D92" s="29"/>
       <c r="E92" s="29" t="s">
@@ -8337,13 +8337,13 @@
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="22" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B96" s="30" t="s">
         <v>395</v>
       </c>
       <c r="C96" s="20" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D96" s="22"/>
       <c r="E96" s="22" t="s">
@@ -8362,13 +8362,13 @@
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="22" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B97" s="30" t="s">
         <v>395</v>
       </c>
       <c r="C97" s="20" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D97" s="22"/>
       <c r="E97" s="22" t="s">
@@ -8387,13 +8387,13 @@
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="22" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B98" s="30" t="s">
         <v>395</v>
       </c>
       <c r="C98" s="20" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D98" s="22"/>
       <c r="E98" s="22" t="s">
@@ -8412,13 +8412,13 @@
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="22" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B99" s="30" t="s">
         <v>395</v>
       </c>
       <c r="C99" s="20" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D99" s="22"/>
       <c r="E99" s="22" t="s">
@@ -8437,13 +8437,13 @@
     </row>
     <row r="100" spans="1:9">
       <c r="A100" s="22" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B100" s="30" t="s">
         <v>395</v>
       </c>
       <c r="C100" s="20" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="D100" s="22"/>
       <c r="E100" s="22" t="s">
@@ -8543,7 +8543,7 @@
         <v>396</v>
       </c>
       <c r="C104" s="20" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D104" s="29"/>
       <c r="E104" s="29" t="s">
@@ -8568,7 +8568,7 @@
         <v>396</v>
       </c>
       <c r="C105" s="20" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="D105" s="29"/>
       <c r="E105" s="29" t="s">
@@ -8612,13 +8612,13 @@
     </row>
     <row r="107" spans="1:9">
       <c r="A107" s="22" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B107" s="30" t="s">
         <v>396</v>
       </c>
       <c r="C107" s="20" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D107" s="22"/>
       <c r="E107" s="22" t="s">
@@ -8637,13 +8637,13 @@
     </row>
     <row r="108" spans="1:9">
       <c r="A108" s="22" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B108" s="30" t="s">
         <v>396</v>
       </c>
       <c r="C108" s="20" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D108" s="22"/>
       <c r="E108" s="22" t="s">
@@ -8662,13 +8662,13 @@
     </row>
     <row r="109" spans="1:9">
       <c r="A109" s="22" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B109" s="30" t="s">
         <v>396</v>
       </c>
       <c r="C109" s="20" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D109" s="22"/>
       <c r="E109" s="22" t="s">
@@ -8687,13 +8687,13 @@
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="22" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B110" s="30" t="s">
         <v>396</v>
       </c>
       <c r="C110" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D110" s="22"/>
       <c r="E110" s="22" t="s">
@@ -8712,13 +8712,13 @@
     </row>
     <row r="111" spans="1:9">
       <c r="A111" s="22" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B111" s="30" t="s">
         <v>396</v>
       </c>
       <c r="C111" s="20" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="D111" s="22"/>
       <c r="E111" s="22" t="s">
@@ -8818,7 +8818,7 @@
         <v>397</v>
       </c>
       <c r="C115" s="20" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="29" t="s">
@@ -8843,7 +8843,7 @@
         <v>397</v>
       </c>
       <c r="C116" s="20" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="29" t="s">
@@ -8887,13 +8887,13 @@
     </row>
     <row r="118" spans="1:9">
       <c r="A118" s="22" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B118" s="30" t="s">
         <v>397</v>
       </c>
       <c r="C118" s="20" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D118" s="22"/>
       <c r="E118" s="22" t="s">
@@ -8912,13 +8912,13 @@
     </row>
     <row r="119" spans="1:9">
       <c r="A119" s="22" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B119" s="30" t="s">
         <v>397</v>
       </c>
       <c r="C119" s="20" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D119" s="22"/>
       <c r="E119" s="22" t="s">
@@ -8937,13 +8937,13 @@
     </row>
     <row r="120" spans="1:9">
       <c r="A120" s="22" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B120" s="30" t="s">
         <v>397</v>
       </c>
       <c r="C120" s="20" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D120" s="22"/>
       <c r="E120" s="22" t="s">
@@ -8962,13 +8962,13 @@
     </row>
     <row r="121" spans="1:9">
       <c r="A121" s="22" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B121" s="30" t="s">
         <v>397</v>
       </c>
       <c r="C121" s="20" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D121" s="22"/>
       <c r="E121" s="22" t="s">
@@ -8987,13 +8987,13 @@
     </row>
     <row r="122" spans="1:9">
       <c r="A122" s="22" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B122" s="30" t="s">
         <v>397</v>
       </c>
       <c r="C122" s="20" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D122" s="22"/>
       <c r="E122" s="22" t="s">
@@ -9043,7 +9043,7 @@
         <v>398</v>
       </c>
       <c r="C124" s="20" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="D124" s="29"/>
       <c r="E124" s="29" t="s">
@@ -9093,7 +9093,7 @@
         <v>398</v>
       </c>
       <c r="C126" s="20" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="D126" s="29"/>
       <c r="E126" s="29" t="s">
@@ -9118,7 +9118,7 @@
         <v>398</v>
       </c>
       <c r="C127" s="20" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D127" s="29"/>
       <c r="E127" s="29" t="s">
@@ -9137,13 +9137,13 @@
     </row>
     <row r="128" spans="1:9" ht="30">
       <c r="A128" s="22" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B128" s="30" t="s">
         <v>398</v>
       </c>
       <c r="C128" s="20" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="D128" s="29"/>
       <c r="E128" s="22" t="s">
@@ -9187,13 +9187,13 @@
     </row>
     <row r="130" spans="1:9" ht="30">
       <c r="A130" s="22" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B130" s="30" t="s">
         <v>398</v>
       </c>
       <c r="C130" s="20" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D130" s="22"/>
       <c r="E130" s="22" t="s">
@@ -9212,13 +9212,13 @@
     </row>
     <row r="131" spans="1:9" ht="30">
       <c r="A131" s="22" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B131" s="30" t="s">
         <v>398</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D131" s="22"/>
       <c r="E131" s="22" t="s">
@@ -9237,13 +9237,13 @@
     </row>
     <row r="132" spans="1:9" ht="30">
       <c r="A132" s="22" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B132" s="30" t="s">
         <v>398</v>
       </c>
       <c r="C132" s="20" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D132" s="22"/>
       <c r="E132" s="22" t="s">
@@ -9262,13 +9262,13 @@
     </row>
     <row r="133" spans="1:9" ht="30">
       <c r="A133" s="22" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B133" s="30" t="s">
         <v>398</v>
       </c>
       <c r="C133" s="20" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D133" s="22"/>
       <c r="E133" s="22" t="s">
@@ -9287,13 +9287,13 @@
     </row>
     <row r="134" spans="1:9" ht="30">
       <c r="A134" s="22" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B134" s="30" t="s">
         <v>398</v>
       </c>
       <c r="C134" s="20" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="D134" s="36"/>
       <c r="E134" s="22" t="s">
@@ -9393,7 +9393,7 @@
         <v>399</v>
       </c>
       <c r="C138" s="20" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D138" s="29"/>
       <c r="E138" s="29" t="s">
@@ -9418,7 +9418,7 @@
         <v>399</v>
       </c>
       <c r="C139" s="20" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D139" s="29"/>
       <c r="E139" s="29" t="s">
@@ -9537,13 +9537,13 @@
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="22" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B144" s="30" t="s">
         <v>399</v>
       </c>
       <c r="C144" s="20" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D144" s="22"/>
       <c r="E144" s="22" t="s">
@@ -9562,13 +9562,13 @@
     </row>
     <row r="145" spans="1:9">
       <c r="A145" s="22" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B145" s="30" t="s">
         <v>399</v>
       </c>
       <c r="C145" s="20" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D145" s="22"/>
       <c r="E145" s="22" t="s">
@@ -9587,13 +9587,13 @@
     </row>
     <row r="146" spans="1:9">
       <c r="A146" s="22" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B146" s="30" t="s">
         <v>399</v>
       </c>
       <c r="C146" s="20" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D146" s="22"/>
       <c r="E146" s="22" t="s">
@@ -9612,13 +9612,13 @@
     </row>
     <row r="147" spans="1:9">
       <c r="A147" s="22" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B147" s="30" t="s">
         <v>399</v>
       </c>
       <c r="C147" s="20" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D147" s="22"/>
       <c r="E147" s="22" t="s">
@@ -9637,13 +9637,13 @@
     </row>
     <row r="148" spans="1:9">
       <c r="A148" s="22" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B148" s="30" t="s">
         <v>399</v>
       </c>
       <c r="C148" s="20" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="D148" s="36"/>
       <c r="E148" s="22" t="s">
@@ -9768,7 +9768,7 @@
         <v>400</v>
       </c>
       <c r="C153" s="20" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D153" s="29"/>
       <c r="E153" s="29" t="s">
@@ -9793,7 +9793,7 @@
         <v>400</v>
       </c>
       <c r="C154" s="20" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D154" s="29"/>
       <c r="E154" s="29" t="s">
@@ -9837,13 +9837,13 @@
     </row>
     <row r="156" spans="1:9">
       <c r="A156" s="22" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B156" s="30" t="s">
         <v>400</v>
       </c>
       <c r="C156" s="20" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D156" s="22"/>
       <c r="E156" s="22" t="s">
@@ -9862,13 +9862,13 @@
     </row>
     <row r="157" spans="1:9">
       <c r="A157" s="22" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B157" s="30" t="s">
         <v>400</v>
       </c>
       <c r="C157" s="20" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D157" s="22"/>
       <c r="E157" s="22" t="s">
@@ -9887,13 +9887,13 @@
     </row>
     <row r="158" spans="1:9">
       <c r="A158" s="22" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B158" s="30" t="s">
         <v>400</v>
       </c>
       <c r="C158" s="20" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D158" s="22"/>
       <c r="E158" s="22" t="s">
@@ -9912,13 +9912,13 @@
     </row>
     <row r="159" spans="1:9">
       <c r="A159" s="22" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B159" s="30" t="s">
         <v>400</v>
       </c>
       <c r="C159" s="20" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D159" s="22"/>
       <c r="E159" s="22" t="s">
@@ -9937,13 +9937,13 @@
     </row>
     <row r="160" spans="1:9">
       <c r="A160" s="22" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B160" s="30" t="s">
         <v>400</v>
       </c>
       <c r="C160" s="20" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="D160" s="36"/>
       <c r="E160" s="22" t="s">
@@ -10043,7 +10043,7 @@
         <v>401</v>
       </c>
       <c r="C164" s="20" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D164" s="29"/>
       <c r="E164" s="29" t="s">
@@ -10068,7 +10068,7 @@
         <v>401</v>
       </c>
       <c r="C165" s="20" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="D165" s="29"/>
       <c r="E165" s="29" t="s">
@@ -10137,13 +10137,13 @@
     </row>
     <row r="168" spans="1:9" ht="30">
       <c r="A168" s="22" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B168" s="30" t="s">
         <v>401</v>
       </c>
       <c r="C168" s="20" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D168" s="22"/>
       <c r="E168" s="22" t="s">
@@ -10162,13 +10162,13 @@
     </row>
     <row r="169" spans="1:9" ht="30">
       <c r="A169" s="22" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B169" s="30" t="s">
         <v>401</v>
       </c>
       <c r="C169" s="20" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D169" s="22"/>
       <c r="E169" s="22" t="s">
@@ -10187,13 +10187,13 @@
     </row>
     <row r="170" spans="1:9" ht="30">
       <c r="A170" s="22" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B170" s="30" t="s">
         <v>401</v>
       </c>
       <c r="C170" s="20" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D170" s="22"/>
       <c r="E170" s="22" t="s">
@@ -10212,13 +10212,13 @@
     </row>
     <row r="171" spans="1:9" ht="30">
       <c r="A171" s="22" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B171" s="30" t="s">
         <v>401</v>
       </c>
       <c r="C171" s="20" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D171" s="22"/>
       <c r="E171" s="22" t="s">
@@ -10237,13 +10237,13 @@
     </row>
     <row r="172" spans="1:9" ht="30">
       <c r="A172" s="22" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B172" s="30" t="s">
         <v>401</v>
       </c>
       <c r="C172" s="20" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D172" s="36"/>
       <c r="E172" s="22" t="s">
@@ -10268,7 +10268,7 @@
         <v>402</v>
       </c>
       <c r="C173" s="20" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="D173" s="29"/>
       <c r="E173" s="29" t="s">
@@ -10387,13 +10387,13 @@
     </row>
     <row r="178" spans="1:9" ht="30">
       <c r="A178" s="22" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B178" s="30" t="s">
         <v>402</v>
       </c>
       <c r="C178" s="20" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="D178" s="22"/>
       <c r="E178" s="22" t="s">
@@ -10412,13 +10412,13 @@
     </row>
     <row r="179" spans="1:9" ht="30">
       <c r="A179" s="22" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B179" s="30" t="s">
         <v>402</v>
       </c>
       <c r="C179" s="20" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D179" s="22"/>
       <c r="E179" s="22" t="s">
@@ -10437,13 +10437,13 @@
     </row>
     <row r="180" spans="1:9" ht="30">
       <c r="A180" s="22" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B180" s="30" t="s">
         <v>402</v>
       </c>
       <c r="C180" s="20" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D180" s="22"/>
       <c r="E180" s="22" t="s">
@@ -10462,13 +10462,13 @@
     </row>
     <row r="181" spans="1:9" ht="30">
       <c r="A181" s="22" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B181" s="30" t="s">
         <v>402</v>
       </c>
       <c r="C181" s="20" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D181" s="22"/>
       <c r="E181" s="22" t="s">
@@ -10487,13 +10487,13 @@
     </row>
     <row r="182" spans="1:9" ht="30">
       <c r="A182" s="22" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B182" s="30" t="s">
         <v>402</v>
       </c>
       <c r="C182" s="20" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="D182" s="36"/>
       <c r="E182" s="22" t="s">
@@ -10543,7 +10543,7 @@
         <v>403</v>
       </c>
       <c r="C184" s="20" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="D184" s="29"/>
       <c r="E184" s="29" t="s">
@@ -10593,7 +10593,7 @@
         <v>403</v>
       </c>
       <c r="C186" s="20" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="D186" s="29"/>
       <c r="E186" s="29" t="s">
@@ -10618,7 +10618,7 @@
         <v>403</v>
       </c>
       <c r="C187" s="20" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="D187" s="29"/>
       <c r="E187" s="29" t="s">
@@ -10662,13 +10662,13 @@
     </row>
     <row r="189" spans="1:9" ht="30">
       <c r="A189" s="22" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B189" s="30" t="s">
         <v>403</v>
       </c>
       <c r="C189" s="20" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D189" s="22"/>
       <c r="E189" s="22" t="s">
@@ -10687,13 +10687,13 @@
     </row>
     <row r="190" spans="1:9" ht="30">
       <c r="A190" s="22" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B190" s="30" t="s">
         <v>403</v>
       </c>
       <c r="C190" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D190" s="22"/>
       <c r="E190" s="22" t="s">
@@ -10712,13 +10712,13 @@
     </row>
     <row r="191" spans="1:9">
       <c r="A191" s="22" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B191" s="30" t="s">
         <v>403</v>
       </c>
       <c r="C191" s="20" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D191" s="22"/>
       <c r="E191" s="22" t="s">
@@ -10737,13 +10737,13 @@
     </row>
     <row r="192" spans="1:9">
       <c r="A192" s="22" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B192" s="30" t="s">
         <v>403</v>
       </c>
       <c r="C192" s="20" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D192" s="22"/>
       <c r="E192" s="22" t="s">
@@ -10762,13 +10762,13 @@
     </row>
     <row r="193" spans="1:9">
       <c r="A193" s="22" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B193" s="30" t="s">
         <v>403</v>
       </c>
       <c r="C193" s="20" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D193" s="36"/>
       <c r="E193" s="22" t="s">
@@ -10868,7 +10868,7 @@
         <v>404</v>
       </c>
       <c r="C197" s="20" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D197" s="29"/>
       <c r="E197" s="29" t="s">
@@ -10893,7 +10893,7 @@
         <v>404</v>
       </c>
       <c r="C198" s="20" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D198" s="29"/>
       <c r="E198" s="29" t="s">
@@ -10937,13 +10937,13 @@
     </row>
     <row r="200" spans="1:9">
       <c r="A200" s="22" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B200" s="30" t="s">
         <v>404</v>
       </c>
       <c r="C200" s="20" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D200" s="22"/>
       <c r="E200" s="22" t="s">
@@ -10962,13 +10962,13 @@
     </row>
     <row r="201" spans="1:9">
       <c r="A201" s="22" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B201" s="30" t="s">
         <v>404</v>
       </c>
       <c r="C201" s="20" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D201" s="22"/>
       <c r="E201" s="22" t="s">
@@ -10987,13 +10987,13 @@
     </row>
     <row r="202" spans="1:9">
       <c r="A202" s="22" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B202" s="30" t="s">
         <v>404</v>
       </c>
       <c r="C202" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D202" s="22"/>
       <c r="E202" s="22" t="s">
@@ -11012,13 +11012,13 @@
     </row>
     <row r="203" spans="1:9">
       <c r="A203" s="22" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B203" s="30" t="s">
         <v>404</v>
       </c>
       <c r="C203" s="20" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D203" s="22"/>
       <c r="E203" s="22" t="s">
@@ -11037,13 +11037,13 @@
     </row>
     <row r="204" spans="1:9">
       <c r="A204" s="22" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B204" s="30" t="s">
         <v>404</v>
       </c>
       <c r="C204" s="20" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="D204" s="36"/>
       <c r="E204" s="22" t="s">
@@ -11537,13 +11537,13 @@
     </row>
     <row r="224" spans="1:9" ht="30">
       <c r="A224" s="22" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B224" s="30" t="s">
         <v>405</v>
       </c>
       <c r="C224" s="20" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D224" s="22"/>
       <c r="E224" s="22" t="s">
@@ -11562,13 +11562,13 @@
     </row>
     <row r="225" spans="1:9" ht="30">
       <c r="A225" s="22" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B225" s="30" t="s">
         <v>405</v>
       </c>
       <c r="C225" s="20" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D225" s="22"/>
       <c r="E225" s="22" t="s">
@@ -11587,13 +11587,13 @@
     </row>
     <row r="226" spans="1:9" ht="30">
       <c r="A226" s="22" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B226" s="30" t="s">
         <v>405</v>
       </c>
       <c r="C226" s="20" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D226" s="22"/>
       <c r="E226" s="22" t="s">
@@ -11612,13 +11612,13 @@
     </row>
     <row r="227" spans="1:9" ht="30">
       <c r="A227" s="22" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B227" s="30" t="s">
         <v>405</v>
       </c>
       <c r="C227" s="20" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D227" s="22"/>
       <c r="E227" s="22" t="s">
@@ -11637,13 +11637,13 @@
     </row>
     <row r="228" spans="1:9" ht="30">
       <c r="A228" s="22" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B228" s="30" t="s">
         <v>405</v>
       </c>
       <c r="C228" s="20" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="D228" s="36"/>
       <c r="E228" s="22" t="s">
@@ -11668,7 +11668,7 @@
         <v>406</v>
       </c>
       <c r="C229" s="20" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="D229" s="29"/>
       <c r="E229" s="29" t="s">
@@ -11887,13 +11887,13 @@
     </row>
     <row r="238" spans="1:9" ht="30">
       <c r="A238" s="22" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B238" s="30" t="s">
         <v>406</v>
       </c>
       <c r="C238" s="20" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D238" s="22"/>
       <c r="E238" s="22" t="s">
@@ -11912,13 +11912,13 @@
     </row>
     <row r="239" spans="1:9" ht="30">
       <c r="A239" s="22" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B239" s="30" t="s">
         <v>406</v>
       </c>
       <c r="C239" s="20" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D239" s="22"/>
       <c r="E239" s="22" t="s">
@@ -11937,13 +11937,13 @@
     </row>
     <row r="240" spans="1:9" ht="30">
       <c r="A240" s="22" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B240" s="30" t="s">
         <v>406</v>
       </c>
       <c r="C240" s="20" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D240" s="22"/>
       <c r="E240" s="22" t="s">
@@ -11962,13 +11962,13 @@
     </row>
     <row r="241" spans="1:9" ht="30">
       <c r="A241" s="22" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B241" s="30" t="s">
         <v>406</v>
       </c>
       <c r="C241" s="20" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D241" s="22"/>
       <c r="E241" s="22" t="s">
@@ -11987,13 +11987,13 @@
     </row>
     <row r="242" spans="1:9" ht="30">
       <c r="A242" s="22" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B242" s="30" t="s">
         <v>406</v>
       </c>
       <c r="C242" s="20" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="D242" s="36"/>
       <c r="E242" s="22" t="s">
@@ -12187,13 +12187,13 @@
     </row>
     <row r="250" spans="1:9" ht="30">
       <c r="A250" s="22" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B250" s="30" t="s">
         <v>407</v>
       </c>
       <c r="C250" s="20" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D250" s="22"/>
       <c r="E250" s="22" t="s">
@@ -12212,13 +12212,13 @@
     </row>
     <row r="251" spans="1:9" ht="30">
       <c r="A251" s="22" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B251" s="30" t="s">
         <v>407</v>
       </c>
       <c r="C251" s="20" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D251" s="22"/>
       <c r="E251" s="22" t="s">
@@ -12237,13 +12237,13 @@
     </row>
     <row r="252" spans="1:9" ht="30">
       <c r="A252" s="22" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B252" s="30" t="s">
         <v>407</v>
       </c>
       <c r="C252" s="20" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D252" s="22"/>
       <c r="E252" s="22" t="s">
@@ -12262,13 +12262,13 @@
     </row>
     <row r="253" spans="1:9" ht="30">
       <c r="A253" s="22" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B253" s="30" t="s">
         <v>407</v>
       </c>
       <c r="C253" s="20" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D253" s="22"/>
       <c r="E253" s="22" t="s">
@@ -12287,13 +12287,13 @@
     </row>
     <row r="254" spans="1:9" ht="30">
       <c r="A254" s="22" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B254" s="30" t="s">
         <v>407</v>
       </c>
       <c r="C254" s="20" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="D254" s="36"/>
       <c r="E254" s="22" t="s">
@@ -12318,7 +12318,7 @@
         <v>408</v>
       </c>
       <c r="C255" s="20" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="D255" s="29"/>
       <c r="E255" s="29" t="s">
@@ -12466,13 +12466,13 @@
     </row>
     <row r="261" spans="1:9" ht="30">
       <c r="A261" s="22" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B261" s="30" t="s">
         <v>408</v>
       </c>
       <c r="C261" s="20" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D261" s="22"/>
       <c r="E261" s="22" t="s">
@@ -12491,13 +12491,13 @@
     </row>
     <row r="262" spans="1:9" ht="30">
       <c r="A262" s="22" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B262" s="30" t="s">
         <v>408</v>
       </c>
       <c r="C262" s="20" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D262" s="22"/>
       <c r="E262" s="22" t="s">
@@ -12516,13 +12516,13 @@
     </row>
     <row r="263" spans="1:9" ht="30">
       <c r="A263" s="22" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B263" s="30" t="s">
         <v>408</v>
       </c>
       <c r="C263" s="20" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D263" s="22"/>
       <c r="E263" s="22" t="s">
@@ -12541,13 +12541,13 @@
     </row>
     <row r="264" spans="1:9" ht="30">
       <c r="A264" s="22" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B264" s="30" t="s">
         <v>408</v>
       </c>
       <c r="C264" s="20" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D264" s="22"/>
       <c r="E264" s="22" t="s">
@@ -12566,13 +12566,13 @@
     </row>
     <row r="265" spans="1:9" ht="30">
       <c r="A265" s="22" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B265" s="30" t="s">
         <v>408</v>
       </c>
       <c r="C265" s="20" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="D265" s="36"/>
       <c r="E265" s="22" t="s">
@@ -12622,7 +12622,7 @@
         <v>409</v>
       </c>
       <c r="C267" s="20" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="D267" s="29"/>
       <c r="E267" s="29" t="s">
@@ -12641,13 +12641,13 @@
     </row>
     <row r="268" spans="1:9">
       <c r="A268" s="22" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B268" s="30" t="s">
         <v>409</v>
       </c>
       <c r="C268" s="20" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="D268" s="36"/>
       <c r="E268" s="29" t="s">
@@ -12820,13 +12820,13 @@
     </row>
     <row r="275" spans="1:9" ht="30">
       <c r="A275" s="22" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B275" s="30" t="s">
         <v>410</v>
       </c>
       <c r="C275" s="20" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D275" s="22"/>
       <c r="E275" s="22" t="s">
@@ -12845,13 +12845,13 @@
     </row>
     <row r="276" spans="1:9" ht="30">
       <c r="A276" s="22" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B276" s="30" t="s">
         <v>410</v>
       </c>
       <c r="C276" s="20" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D276" s="22"/>
       <c r="E276" s="22" t="s">
@@ -12870,13 +12870,13 @@
     </row>
     <row r="277" spans="1:9" ht="30">
       <c r="A277" s="22" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B277" s="30" t="s">
         <v>410</v>
       </c>
       <c r="C277" s="20" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D277" s="22"/>
       <c r="E277" s="22" t="s">
@@ -12895,13 +12895,13 @@
     </row>
     <row r="278" spans="1:9" ht="30">
       <c r="A278" s="22" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B278" s="30" t="s">
         <v>410</v>
       </c>
       <c r="C278" s="20" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D278" s="22"/>
       <c r="E278" s="22" t="s">
@@ -12920,13 +12920,13 @@
     </row>
     <row r="279" spans="1:9" ht="30">
       <c r="A279" s="22" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B279" s="30" t="s">
         <v>410</v>
       </c>
       <c r="C279" s="20" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D279" s="36"/>
       <c r="E279" s="22" t="s">
@@ -13099,13 +13099,13 @@
     </row>
     <row r="286" spans="1:9" ht="30">
       <c r="A286" s="22" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B286" s="30" t="s">
         <v>411</v>
       </c>
       <c r="C286" s="20" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D286" s="22"/>
       <c r="E286" s="22" t="s">
@@ -13124,13 +13124,13 @@
     </row>
     <row r="287" spans="1:9" ht="30">
       <c r="A287" s="22" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B287" s="30" t="s">
         <v>411</v>
       </c>
       <c r="C287" s="20" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D287" s="22"/>
       <c r="E287" s="22" t="s">
@@ -13149,13 +13149,13 @@
     </row>
     <row r="288" spans="1:9" ht="30">
       <c r="A288" s="22" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B288" s="30" t="s">
         <v>411</v>
       </c>
       <c r="C288" s="20" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D288" s="22"/>
       <c r="E288" s="22" t="s">
@@ -13174,13 +13174,13 @@
     </row>
     <row r="289" spans="1:9" ht="30">
       <c r="A289" s="22" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B289" s="30" t="s">
         <v>411</v>
       </c>
       <c r="C289" s="20" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D289" s="22"/>
       <c r="E289" s="22" t="s">
@@ -13199,13 +13199,13 @@
     </row>
     <row r="290" spans="1:9" ht="30">
       <c r="A290" s="22" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B290" s="30" t="s">
         <v>411</v>
       </c>
       <c r="C290" s="20" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D290" s="36"/>
       <c r="E290" s="22" t="s">
@@ -13230,7 +13230,7 @@
         <v>412</v>
       </c>
       <c r="C291" s="20" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="D291" s="29"/>
       <c r="E291" s="29" t="s">
@@ -13255,7 +13255,7 @@
         <v>412</v>
       </c>
       <c r="C292" s="20" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="D292" s="29"/>
       <c r="E292" s="29" t="s">
@@ -13280,7 +13280,7 @@
         <v>412</v>
       </c>
       <c r="C293" s="20" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="D293" s="29"/>
       <c r="E293" s="29" t="s">
@@ -13355,7 +13355,7 @@
         <v>412</v>
       </c>
       <c r="C296" s="20" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="D296" s="29"/>
       <c r="E296" s="29" t="s">
@@ -13374,13 +13374,13 @@
     </row>
     <row r="297" spans="1:9">
       <c r="A297" s="22" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B297" s="30" t="s">
         <v>412</v>
       </c>
       <c r="C297" s="20" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="D297" s="36"/>
       <c r="E297" s="29" t="s">
@@ -13474,13 +13474,13 @@
     </row>
     <row r="301" spans="1:9" ht="30">
       <c r="A301" s="22" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B301" s="30" t="s">
         <v>413</v>
       </c>
       <c r="C301" s="20" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D301" s="22"/>
       <c r="E301" s="22" t="s">
@@ -13499,13 +13499,13 @@
     </row>
     <row r="302" spans="1:9" ht="30">
       <c r="A302" s="22" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B302" s="30" t="s">
         <v>413</v>
       </c>
       <c r="C302" s="20" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D302" s="22"/>
       <c r="E302" s="22" t="s">
@@ -13524,13 +13524,13 @@
     </row>
     <row r="303" spans="1:9" ht="30">
       <c r="A303" s="22" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B303" s="30" t="s">
         <v>413</v>
       </c>
       <c r="C303" s="20" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D303" s="22"/>
       <c r="E303" s="22" t="s">
@@ -13549,13 +13549,13 @@
     </row>
     <row r="304" spans="1:9" ht="30">
       <c r="A304" s="22" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B304" s="30" t="s">
         <v>413</v>
       </c>
       <c r="C304" s="20" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D304" s="22"/>
       <c r="E304" s="22" t="s">
@@ -13574,13 +13574,13 @@
     </row>
     <row r="305" spans="1:9" ht="30">
       <c r="A305" s="22" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B305" s="30" t="s">
         <v>413</v>
       </c>
       <c r="C305" s="20" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="D305" s="36"/>
       <c r="E305" s="22" t="s">
@@ -13674,13 +13674,13 @@
     </row>
     <row r="309" spans="1:9" ht="30">
       <c r="A309" s="22" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B309" s="30" t="s">
         <v>414</v>
       </c>
       <c r="C309" s="20" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D309" s="22"/>
       <c r="E309" s="22" t="s">
@@ -13699,13 +13699,13 @@
     </row>
     <row r="310" spans="1:9" ht="30">
       <c r="A310" s="22" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B310" s="30" t="s">
         <v>414</v>
       </c>
       <c r="C310" s="20" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D310" s="22"/>
       <c r="E310" s="22" t="s">
@@ -13724,13 +13724,13 @@
     </row>
     <row r="311" spans="1:9" ht="30">
       <c r="A311" s="22" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B311" s="30" t="s">
         <v>414</v>
       </c>
       <c r="C311" s="20" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D311" s="22"/>
       <c r="E311" s="22" t="s">
@@ -13749,13 +13749,13 @@
     </row>
     <row r="312" spans="1:9" ht="30">
       <c r="A312" s="22" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B312" s="30" t="s">
         <v>414</v>
       </c>
       <c r="C312" s="20" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D312" s="22"/>
       <c r="E312" s="22" t="s">
@@ -13774,13 +13774,13 @@
     </row>
     <row r="313" spans="1:9" ht="30">
       <c r="A313" s="22" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B313" s="30" t="s">
         <v>414</v>
       </c>
       <c r="C313" s="20" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D313" s="36"/>
       <c r="E313" s="22" t="s">
@@ -13805,7 +13805,7 @@
         <v>415</v>
       </c>
       <c r="C314" s="20" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="D314" s="29"/>
       <c r="E314" s="29" t="s">
@@ -13949,13 +13949,13 @@
     </row>
     <row r="320" spans="1:9" ht="30">
       <c r="A320" s="22" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B320" s="30" t="s">
         <v>415</v>
       </c>
       <c r="C320" s="20" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D320" s="22"/>
       <c r="E320" s="22" t="s">
@@ -13974,13 +13974,13 @@
     </row>
     <row r="321" spans="1:9" ht="30">
       <c r="A321" s="22" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B321" s="30" t="s">
         <v>415</v>
       </c>
       <c r="C321" s="20" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D321" s="22"/>
       <c r="E321" s="22" t="s">
@@ -13999,13 +13999,13 @@
     </row>
     <row r="322" spans="1:9" ht="30">
       <c r="A322" s="22" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B322" s="30" t="s">
         <v>415</v>
       </c>
       <c r="C322" s="20" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D322" s="22"/>
       <c r="E322" s="22" t="s">
@@ -14024,13 +14024,13 @@
     </row>
     <row r="323" spans="1:9" ht="30">
       <c r="A323" s="22" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B323" s="30" t="s">
         <v>415</v>
       </c>
       <c r="C323" s="20" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D323" s="22"/>
       <c r="E323" s="22" t="s">
@@ -14049,13 +14049,13 @@
     </row>
     <row r="324" spans="1:9" ht="30">
       <c r="A324" s="22" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B324" s="30" t="s">
         <v>415</v>
       </c>
       <c r="C324" s="20" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D324" s="36"/>
       <c r="E324" s="22" t="s">
@@ -14105,7 +14105,7 @@
         <v>416</v>
       </c>
       <c r="C326" s="20" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="D326" s="29"/>
       <c r="E326" s="29" t="s">
@@ -14124,13 +14124,13 @@
     </row>
     <row r="327" spans="1:9">
       <c r="A327" s="22" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B327" s="30" t="s">
         <v>416</v>
       </c>
       <c r="C327" s="20" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="D327" s="36"/>
       <c r="E327" s="29" t="s">
@@ -14303,13 +14303,13 @@
     </row>
     <row r="334" spans="1:9" ht="30">
       <c r="A334" s="22" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B334" s="30" t="s">
         <v>417</v>
       </c>
       <c r="C334" s="20" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="D334" s="22"/>
       <c r="E334" s="22" t="s">
@@ -14328,13 +14328,13 @@
     </row>
     <row r="335" spans="1:9" ht="30">
       <c r="A335" s="22" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B335" s="30" t="s">
         <v>417</v>
       </c>
       <c r="C335" s="20" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D335" s="22"/>
       <c r="E335" s="22" t="s">
@@ -14353,13 +14353,13 @@
     </row>
     <row r="336" spans="1:9" ht="30">
       <c r="A336" s="22" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B336" s="30" t="s">
         <v>417</v>
       </c>
       <c r="C336" s="20" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D336" s="22"/>
       <c r="E336" s="22" t="s">
@@ -14378,13 +14378,13 @@
     </row>
     <row r="337" spans="1:9" ht="30">
       <c r="A337" s="22" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B337" s="30" t="s">
         <v>417</v>
       </c>
       <c r="C337" s="20" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D337" s="22"/>
       <c r="E337" s="22" t="s">
@@ -14403,13 +14403,13 @@
     </row>
     <row r="338" spans="1:9" ht="30">
       <c r="A338" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B338" s="30" t="s">
         <v>417</v>
       </c>
       <c r="C338" s="20" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="D338" s="36"/>
       <c r="E338" s="22" t="s">
@@ -14582,13 +14582,13 @@
     </row>
     <row r="345" spans="1:9" ht="30">
       <c r="A345" s="22" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B345" s="30" t="s">
         <v>418</v>
       </c>
       <c r="C345" s="20" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D345" s="22"/>
       <c r="E345" s="22" t="s">
@@ -14607,13 +14607,13 @@
     </row>
     <row r="346" spans="1:9" ht="30">
       <c r="A346" s="22" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B346" s="30" t="s">
         <v>418</v>
       </c>
       <c r="C346" s="20" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D346" s="22"/>
       <c r="E346" s="22" t="s">
@@ -14632,13 +14632,13 @@
     </row>
     <row r="347" spans="1:9" ht="30">
       <c r="A347" s="22" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B347" s="30" t="s">
         <v>418</v>
       </c>
       <c r="C347" s="20" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D347" s="22"/>
       <c r="E347" s="22" t="s">
@@ -14657,13 +14657,13 @@
     </row>
     <row r="348" spans="1:9" ht="30">
       <c r="A348" s="22" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B348" s="30" t="s">
         <v>418</v>
       </c>
       <c r="C348" s="20" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D348" s="22"/>
       <c r="E348" s="22" t="s">
@@ -14682,13 +14682,13 @@
     </row>
     <row r="349" spans="1:9" ht="30">
       <c r="A349" s="22" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B349" s="30" t="s">
         <v>418</v>
       </c>
       <c r="C349" s="20" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="D349" s="36"/>
       <c r="E349" s="22" t="s">
@@ -14738,7 +14738,7 @@
         <v>31</v>
       </c>
       <c r="C351" s="20" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="D351" s="29"/>
       <c r="E351" s="29" t="s">
@@ -14813,7 +14813,7 @@
         <v>31</v>
       </c>
       <c r="C354" s="20" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D354" s="29"/>
       <c r="E354" s="29" t="s">
@@ -14838,7 +14838,7 @@
         <v>31</v>
       </c>
       <c r="C355" s="20" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D355" s="29"/>
       <c r="E355" s="29" t="s">
@@ -14863,7 +14863,7 @@
         <v>31</v>
       </c>
       <c r="C356" s="20" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D356" s="29"/>
       <c r="E356" s="29" t="s">
@@ -14888,7 +14888,7 @@
         <v>32</v>
       </c>
       <c r="C357" s="20" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D357" s="29"/>
       <c r="E357" s="29" t="s">
@@ -14988,7 +14988,7 @@
         <v>420</v>
       </c>
       <c r="C361" s="20" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D361" s="29"/>
       <c r="E361" s="29" t="s">
@@ -15088,7 +15088,7 @@
         <v>423</v>
       </c>
       <c r="C365" s="20" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="D365" s="29"/>
       <c r="E365" s="29" t="s">
@@ -15688,7 +15688,7 @@
         <v>425</v>
       </c>
       <c r="C389" s="20" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D389" s="29"/>
       <c r="E389" s="29" t="s">
@@ -15713,7 +15713,7 @@
         <v>425</v>
       </c>
       <c r="C390" s="20" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="D390" s="29"/>
       <c r="E390" s="29" t="s">
@@ -15988,7 +15988,7 @@
         <v>426</v>
       </c>
       <c r="C401" s="20" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D401" s="29"/>
       <c r="E401" s="29" t="s">
@@ -16009,13 +16009,13 @@
     </row>
     <row r="402" spans="1:9" ht="30">
       <c r="A402" s="22" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B402" s="30" t="s">
         <v>426</v>
       </c>
       <c r="C402" s="20" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D402" s="36"/>
       <c r="E402" s="29" t="s">
@@ -16090,7 +16090,7 @@
         <v>427</v>
       </c>
       <c r="C405" s="20" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D405" s="29"/>
       <c r="E405" s="29" t="s">
@@ -16240,7 +16240,7 @@
         <v>427</v>
       </c>
       <c r="C411" s="20" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="D411" s="29"/>
       <c r="E411" s="29" t="s">
@@ -16340,7 +16340,7 @@
         <v>427</v>
       </c>
       <c r="C415" s="20" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="D415" s="29"/>
       <c r="E415" s="29" t="s">
@@ -16415,7 +16415,7 @@
         <v>427</v>
       </c>
       <c r="C418" s="20" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D418" s="29"/>
       <c r="E418" s="29" t="s">
@@ -16565,7 +16565,7 @@
         <v>427</v>
       </c>
       <c r="C424" s="20" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="D424" s="29"/>
       <c r="E424" s="29" t="s">
@@ -16665,7 +16665,7 @@
         <v>427</v>
       </c>
       <c r="C428" s="20" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D428" s="29"/>
       <c r="E428" s="29" t="s">
@@ -17115,7 +17115,7 @@
         <v>427</v>
       </c>
       <c r="C446" s="20" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D446" s="29"/>
       <c r="E446" s="29" t="s">
@@ -17140,7 +17140,7 @@
         <v>427</v>
       </c>
       <c r="C447" s="20" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D447" s="29"/>
       <c r="E447" s="29" t="s">
@@ -17165,7 +17165,7 @@
         <v>427</v>
       </c>
       <c r="C448" s="20" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D448" s="29"/>
       <c r="E448" s="29" t="s">
@@ -17190,7 +17190,7 @@
         <v>427</v>
       </c>
       <c r="C449" s="20" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D449" s="29"/>
       <c r="E449" s="29" t="s">
@@ -17215,7 +17215,7 @@
         <v>427</v>
       </c>
       <c r="C450" s="20" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D450" s="29"/>
       <c r="E450" s="29" t="s">
@@ -17240,7 +17240,7 @@
         <v>427</v>
       </c>
       <c r="C451" s="20" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D451" s="29"/>
       <c r="E451" s="29" t="s">
@@ -17265,7 +17265,7 @@
         <v>427</v>
       </c>
       <c r="C452" s="20" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D452" s="29"/>
       <c r="E452" s="29" t="s">
@@ -17290,7 +17290,7 @@
         <v>427</v>
       </c>
       <c r="C453" s="20" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D453" s="29"/>
       <c r="E453" s="29" t="s">
@@ -17315,7 +17315,7 @@
         <v>427</v>
       </c>
       <c r="C454" s="20" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D454" s="29"/>
       <c r="E454" s="29" t="s">
@@ -17340,7 +17340,7 @@
         <v>427</v>
       </c>
       <c r="C455" s="20" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D455" s="29"/>
       <c r="E455" s="29" t="s">
@@ -17365,7 +17365,7 @@
         <v>427</v>
       </c>
       <c r="C456" s="20" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D456" s="29"/>
       <c r="E456" s="29" t="s">
@@ -17390,7 +17390,7 @@
         <v>427</v>
       </c>
       <c r="C457" s="20" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D457" s="29"/>
       <c r="E457" s="29" t="s">
@@ -17415,7 +17415,7 @@
         <v>427</v>
       </c>
       <c r="C458" s="20" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D458" s="29"/>
       <c r="E458" s="29" t="s">
@@ -17440,7 +17440,7 @@
         <v>427</v>
       </c>
       <c r="C459" s="20" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D459" s="29"/>
       <c r="E459" s="29" t="s">
@@ -17465,7 +17465,7 @@
         <v>427</v>
       </c>
       <c r="C460" s="20" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D460" s="29"/>
       <c r="E460" s="29" t="s">
@@ -17490,7 +17490,7 @@
         <v>427</v>
       </c>
       <c r="C461" s="20" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="D461" s="29"/>
       <c r="E461" s="29" t="s">
@@ -17590,7 +17590,7 @@
         <v>428</v>
       </c>
       <c r="C465" s="20" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D465" s="22" t="s">
         <v>682</v>
@@ -17638,13 +17638,13 @@
     </row>
     <row r="467" spans="1:9" ht="30">
       <c r="A467" s="22" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B467" s="30" t="s">
         <v>430</v>
       </c>
       <c r="C467" s="20" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="D467" s="36"/>
       <c r="E467" s="29" t="s">
@@ -17669,7 +17669,7 @@
         <v>430</v>
       </c>
       <c r="C468" s="20" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D468" s="29"/>
       <c r="E468" s="29" t="s">
@@ -17694,7 +17694,7 @@
         <v>430</v>
       </c>
       <c r="C469" s="20" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D469" s="29"/>
       <c r="E469" s="29" t="s">
@@ -17719,7 +17719,7 @@
         <v>430</v>
       </c>
       <c r="C470" s="20" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D470" s="29"/>
       <c r="E470" s="29" t="s">
@@ -17744,7 +17744,7 @@
         <v>430</v>
       </c>
       <c r="C471" s="20" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D471" s="29"/>
       <c r="E471" s="29" t="s">
@@ -17769,7 +17769,7 @@
         <v>430</v>
       </c>
       <c r="C472" s="20" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D472" s="29"/>
       <c r="E472" s="29" t="s">
@@ -17794,7 +17794,7 @@
         <v>430</v>
       </c>
       <c r="C473" s="20" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D473" s="29"/>
       <c r="E473" s="29" t="s">
@@ -17819,7 +17819,7 @@
         <v>430</v>
       </c>
       <c r="C474" s="20" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D474" s="29"/>
       <c r="E474" s="29" t="s">
@@ -17844,7 +17844,7 @@
         <v>430</v>
       </c>
       <c r="C475" s="20" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D475" s="29"/>
       <c r="E475" s="29" t="s">
@@ -17869,7 +17869,7 @@
         <v>430</v>
       </c>
       <c r="C476" s="20" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="D476" s="29"/>
       <c r="E476" s="29" t="s">
@@ -17894,7 +17894,7 @@
         <v>430</v>
       </c>
       <c r="C477" s="20" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="D477" s="29"/>
       <c r="E477" s="29" t="s">
@@ -17919,7 +17919,7 @@
         <v>430</v>
       </c>
       <c r="C478" s="20" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D478" s="29"/>
       <c r="E478" s="29" t="s">
@@ -17944,7 +17944,7 @@
         <v>430</v>
       </c>
       <c r="C479" s="20" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D479" s="29"/>
       <c r="E479" s="29" t="s">
@@ -17969,7 +17969,7 @@
         <v>430</v>
       </c>
       <c r="C480" s="20" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D480" s="29"/>
       <c r="E480" s="29" t="s">
@@ -17994,7 +17994,7 @@
         <v>430</v>
       </c>
       <c r="C481" s="20" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D481" s="29"/>
       <c r="E481" s="29" t="s">
@@ -18019,7 +18019,7 @@
         <v>430</v>
       </c>
       <c r="C482" s="20" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D482" s="29"/>
       <c r="E482" s="29" t="s">
@@ -18044,7 +18044,7 @@
         <v>430</v>
       </c>
       <c r="C483" s="20" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D483" s="29"/>
       <c r="E483" s="29" t="s">
@@ -18069,7 +18069,7 @@
         <v>430</v>
       </c>
       <c r="C484" s="20" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="D484" s="29"/>
       <c r="E484" s="29" t="s">
@@ -18094,7 +18094,7 @@
         <v>430</v>
       </c>
       <c r="C485" s="20" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="D485" s="29"/>
       <c r="E485" s="29" t="s">
@@ -18119,7 +18119,7 @@
         <v>430</v>
       </c>
       <c r="C486" s="20" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D486" s="22"/>
       <c r="E486" s="29" t="s">
@@ -18371,11 +18371,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -18383,6 +18378,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A403:B403 D403:I403 A468:B485 D468:I486 A20:H46 A34:I46 A101:I106 A112:I117 A135:I143 A149:I155 A173:I177 A183:I188 A194:I199 A205:I223 A229:I237 A243:I249 A255:I260 A280:I285 A306:I308 A314:I319 A339:I344 A65:I77 A83:I95 A161:I167 A47:B51 A96:B100 A78:B82 A60:B64 A52:I59 A118:B122 A107:B111 A130:B134 A144:B148 A156:B160 A168:B172 A178:B182 A189:B193 A200:B204 A224:B228 A238:B242 A250:B254 A261:B265 A266:I274 A275:B279 A286:B290 A291:I300 A301:B305 A309:B313 A320:B324 A325:I333 A334:B338 A345:B349 A350:I402 A487:I495 A404:I467 A123:I129 I20:I495">
@@ -19467,7 +19467,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B468:B488 C3 B19:B50 B52:B55 B57:B63 B65:B81 B83:B99 B112:B121 B101:B110 B123:B125 B126:B133 B135:B147 B149:B159 B161:B171 B173:B181 B183:B192 B194:B203 B205:B227 B229:B241 B243:B253 B255:B264 B266:B267 B269:B278 B280:B289 B291:B296 B298:B304 B306:B312 B314:B323 B325:B326 B328:B337 B339:B348 B350:B401 B403:B466 B489:B497" numberStoredAsText="1"/>
+    <ignoredError sqref="B468:B488 B19:B50 B52:B55 B57:B63 B65:B81 B83:B99 B112:B121 B101:B110 B123:B125 B126:B133 B135:B147 B149:B159 B161:B171 B173:B181 B183:B192 B194:B203 B205:B227 B229:B241 B243:B253 B255:B264 B266:B267 B269:B278 B280:B289 B291:B296 B298:B304 B306:B312 B314:B323 B325:B326 B328:B337 B339:B348 B350:B401 B403:B466 B489:B497" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -19477,6 +19477,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -19525,32 +19540,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19564,15 +19563,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>